<commit_message>
Commit inicial do projeto
</commit_message>
<xml_diff>
--- a/resultados_processos.xlsx
+++ b/resultados_processos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,11 +460,41 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0015765-24.2016.4.01.3803</t>
+          <t>1004944-53.2023.4.06.3804</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>agravo3.pdf</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0001547-36.2008.4.01.3814</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>agravo4.pdf</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>5064477-98.2024.8.13.0702</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
reorganiza estrutura para deploy
</commit_message>
<xml_diff>
--- a/resultados_processos.xlsx
+++ b/resultados_processos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>agravo1.pdf</t>
+          <t>agravo3.pdf</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -449,52 +449,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1000301-04.2023.4.06.3820</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>agravo2.pdf</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>1004944-53.2023.4.06.3804</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>agravo3.pdf</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
           <t>0001547-36.2008.4.01.3814</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>agravo4.pdf</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>5064477-98.2024.8.13.0702</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Tornar layout responsivo para dispositivos móveis
</commit_message>
<xml_diff>
--- a/resultados_processos.xlsx
+++ b/resultados_processos.xlsx
@@ -441,7 +441,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>agravo3.pdf</t>
+          <t>00410000248202424_agravo1.pdf</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -449,7 +449,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0001547-36.2008.4.01.3814</t>
+          <t>0000002-95.2017.4.01.3819</t>
         </is>
       </c>
     </row>

</xml_diff>